<commit_message>
Added new test test_product_page.py and new dependents.
</commit_message>
<xml_diff>
--- a/Zhelp.xlsx
+++ b/Zhelp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IDEA" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Что такое Page Object Model?</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>Метод возвращающий Страницу логина.</t>
+  </si>
+  <si>
+    <t>У нас наследование идет о BasePage для ProductPage примеры</t>
   </si>
 </sst>
 </file>
@@ -723,7 +726,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AB8B29B-3253-4945-AE7B-497D811401E0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB8B29B-3253-4945-AE7B-497D811401E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -779,6 +782,163 @@
         <a:xfrm>
           <a:off x="0" y="4381500"/>
           <a:ext cx="11342857" cy="3590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5885714</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>56833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2647950"/>
+          <a:ext cx="5885714" cy="2533333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5600000</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5924550"/>
+          <a:ext cx="5600000" cy="3676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5866667</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>132881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9696450"/>
+          <a:ext cx="5866667" cy="3752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6705600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>484570</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>28025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Рисунок 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="7610475"/>
+          <a:ext cx="9638095" cy="4400000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1055,7 +1215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
@@ -1344,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,8 +1535,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added mark login_guest and class test_main_page in test
</commit_message>
<xml_diff>
--- a/Zhelp.xlsx
+++ b/Zhelp.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B549FC9F-8DCC-4A44-97EE-AA081E21CF79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDEA" sheetId="2" r:id="rId1"/>
     <sheet name="Page Object Model" sheetId="1" r:id="rId2"/>
+    <sheet name="setup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>Что такое Page Object Model?</t>
   </si>
@@ -515,13 +517,73 @@
   </si>
   <si>
     <t>У нас наследование идет о BasePage для ProductPage примеры</t>
+  </si>
+  <si>
+    <t>@pytest.mark.add_to_basket</t>
+  </si>
+  <si>
+    <t>class TestAddToBasketFromProductPage(object):</t>
+  </si>
+  <si>
+    <t>    @pytest.fixture(scope="function", autouse=True)</t>
+  </si>
+  <si>
+    <t>    def setup(self):</t>
+  </si>
+  <si>
+    <t>        self.product = ProductFactory(title="Best book created by robot")</t>
+  </si>
+  <si>
+    <t>        self.link = self.product.link</t>
+  </si>
+  <si>
+    <t>        yield</t>
+  </si>
+  <si>
+    <t>        self.product.delete()</t>
+  </si>
+  <si>
+    <t>    def test_guest_cant_see_success_message(self, browser):</t>
+  </si>
+  <si>
+    <t>        page = ProductPage(browser, self.link)</t>
+  </si>
+  <si>
+    <t>Метка добавить в карзину(вызвать можно через консоль данный метод)</t>
+  </si>
+  <si>
+    <t>Название класса</t>
+  </si>
+  <si>
+    <t>фикстура с автозапуском для тестов</t>
+  </si>
+  <si>
+    <t>добавление сетапа</t>
+  </si>
+  <si>
+    <t>Добавление продукта с названием таким то</t>
+  </si>
+  <si>
+    <t>установка ссылки для продукта</t>
+  </si>
+  <si>
+    <t>По завершению тест</t>
+  </si>
+  <si>
+    <t>удаляем продукт из бд или функцией</t>
+  </si>
+  <si>
+    <t>начало теста передаем селф и бруезер</t>
+  </si>
+  <si>
+    <t>создание страницы Продукта</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,6 +663,13 @@
       <family val="3"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -652,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
@@ -688,6 +757,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,7 +798,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB8B29B-3253-4945-AE7B-497D811401E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -767,7 +839,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -810,7 +888,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -848,7 +932,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -886,7 +976,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -924,7 +1020,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4"/>
+        <xdr:cNvPr id="5" name="Рисунок 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1212,35 +1314,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="59.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
@@ -1262,87 +1364,87 @@
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D44" s="9" t="s">
         <v>25</v>
       </c>
@@ -1355,7 +1457,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D45" s="11" t="s">
         <v>26</v>
       </c>
@@ -1365,7 +1467,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D46" s="11" t="s">
         <v>27</v>
       </c>
@@ -1375,7 +1477,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D47" s="11" t="s">
         <v>28</v>
       </c>
@@ -1385,7 +1487,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D48" s="11" t="s">
         <v>29</v>
       </c>
@@ -1395,7 +1497,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D49" s="11" t="s">
         <v>30</v>
       </c>
@@ -1405,7 +1507,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
     </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D50" s="12"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -1413,7 +1515,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D51" s="7" t="s">
         <v>31</v>
       </c>
@@ -1426,7 +1528,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D52" s="7" t="s">
         <v>32</v>
       </c>
@@ -1436,7 +1538,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D53" s="8"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -1444,7 +1546,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D54" s="13" t="s">
         <v>26</v>
       </c>
@@ -1457,7 +1559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D55" s="15" t="s">
         <v>33</v>
       </c>
@@ -1467,7 +1569,7 @@
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
     </row>
-    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D56" s="15" t="s">
         <v>28</v>
       </c>
@@ -1477,7 +1579,7 @@
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
     </row>
-    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D57" s="15" t="s">
         <v>34</v>
       </c>
@@ -1487,7 +1589,7 @@
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
     </row>
-    <row r="58" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
@@ -1503,39 +1605,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="164.7109375" customWidth="1"/>
+    <col min="1" max="1" width="164.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1545,4 +1647,103 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F57B42-CB98-4688-83BA-73B965274CC0}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="55.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added change Help files
</commit_message>
<xml_diff>
--- a/Zhelp.xlsx
+++ b/Zhelp.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686303F8-88A3-4675-B7D4-F2ED5ACCAD8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="IDEA" sheetId="2" r:id="rId1"/>
-    <sheet name="Page Object Model" sheetId="1" r:id="rId2"/>
-    <sheet name="setup" sheetId="3" r:id="rId3"/>
-    <sheet name="От пользователя " sheetId="4" r:id="rId4"/>
+    <sheet name="YouTybe" sheetId="6" r:id="rId1"/>
+    <sheet name="IDEA" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="5" r:id="rId3"/>
+    <sheet name="Page Object Model" sheetId="1" r:id="rId4"/>
+    <sheet name="setup" sheetId="3" r:id="rId5"/>
+    <sheet name="От пользователя " sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>Что такое Page Object Model?</t>
   </si>
@@ -767,11 +770,14 @@
   <si>
     <t>И откуда взялся тест test_guest_can_add_product_to_basket?</t>
   </si>
+  <si>
+    <t>https://youtu.be/UoGyLbfs05o</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1008,7 +1014,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1052,7 +1058,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1101,7 +1107,7 @@
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1145,7 +1151,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1189,7 +1195,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1233,7 +1239,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1524,35 +1530,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7577C05-B140-4972-8F27-F7347616D4B5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="59.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
@@ -1574,87 +1601,87 @@
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D44" s="9" t="s">
         <v>25</v>
       </c>
@@ -1667,7 +1694,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D45" s="11" t="s">
         <v>26</v>
       </c>
@@ -1677,7 +1704,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D46" s="11" t="s">
         <v>27</v>
       </c>
@@ -1687,7 +1714,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D47" s="11" t="s">
         <v>28</v>
       </c>
@@ -1697,7 +1724,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D48" s="11" t="s">
         <v>29</v>
       </c>
@@ -1707,7 +1734,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D49" s="11" t="s">
         <v>30</v>
       </c>
@@ -1717,7 +1744,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
     </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D50" s="12"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -1725,7 +1752,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D51" s="7" t="s">
         <v>31</v>
       </c>
@@ -1738,7 +1765,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D52" s="7" t="s">
         <v>32</v>
       </c>
@@ -1748,7 +1775,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D53" s="8"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -1756,7 +1783,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D54" s="13" t="s">
         <v>26</v>
       </c>
@@ -1769,7 +1796,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D55" s="15" t="s">
         <v>33</v>
       </c>
@@ -1779,7 +1806,7 @@
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
     </row>
-    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D56" s="15" t="s">
         <v>28</v>
       </c>
@@ -1789,7 +1816,7 @@
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
     </row>
-    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D57" s="15" t="s">
         <v>34</v>
       </c>
@@ -1799,7 +1826,7 @@
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
     </row>
-    <row r="58" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
@@ -1814,40 +1841,52 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42A3F48-4A83-484F-AA24-3F9E29AE9EBF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="164.7109375" customWidth="1"/>
+    <col min="1" max="1" width="164.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1859,20 +1898,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>39</v>
       </c>
@@ -1880,7 +1919,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>40</v>
       </c>
@@ -1888,7 +1927,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>41</v>
       </c>
@@ -1896,7 +1935,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>42</v>
       </c>
@@ -1904,7 +1943,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>43</v>
       </c>
@@ -1912,7 +1951,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +1959,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>45</v>
       </c>
@@ -1928,7 +1967,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>46</v>
       </c>
@@ -1936,7 +1975,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>47</v>
       </c>
@@ -1944,7 +1983,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>48</v>
       </c>
@@ -1958,150 +1997,150 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="92.28515625" customWidth="1"/>
+    <col min="1" max="1" width="92.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>85</v>
       </c>

</xml_diff>